<commit_message>
Missing example, error, and notes for BaseUrl variable
</commit_message>
<xml_diff>
--- a/Documentation/Environment variables.xlsx
+++ b/Documentation/Environment variables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkrystyan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkrystyan\Desktop\NotifyNL-OMC-Obfuscated\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F0DA51-7B71-476E-82F4-75E8618AE2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E708C960-C38C-45F4-903F-C0BF45BB2D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{120E288B-D946-4194-8F61-91138CA40827}"/>
+    <workbookView xWindow="-28020" yWindow="795" windowWidth="21600" windowHeight="11325" xr2:uid="{120E288B-D946-4194-8F61-91138CA40827}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="71">
   <si>
     <t>Variable value</t>
   </si>
@@ -307,13 +307,19 @@
   </si>
   <si>
     <t>You have to use the domain part from URLs where you are hosting the dedicated Open services</t>
+  </si>
+  <si>
+    <t>https://www.test.something.com</t>
+  </si>
+  <si>
+    <t>The domain where your Notify NL is deployed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,6 +347,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -396,14 +410,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -417,17 +429,24 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -742,67 +761,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D356E4BC-09A1-470E-86C2-E2ED07724CC6}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="87.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="96" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="87.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="96" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -810,17 +829,17 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -828,17 +847,17 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -846,17 +865,17 @@
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>60</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -864,76 +883,85 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="8"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" s="4" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" s="3" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" s="4" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="3" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -941,17 +969,17 @@
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="2" t="s">
+      <c r="E13" s="7"/>
+      <c r="F13" s="1" t="s">
         <v>39</v>
       </c>
     </row>
@@ -959,17 +987,17 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="2" t="s">
+      <c r="E14" s="7"/>
+      <c r="F14" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -977,17 +1005,17 @@
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>60</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="8" t="s">
+      <c r="E15" s="7"/>
+      <c r="F15" s="6" t="s">
         <v>65</v>
       </c>
     </row>
@@ -995,58 +1023,58 @@
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="8"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" s="3" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="B19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1054,46 +1082,46 @@
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="4" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+    <row r="21" spans="1:6" s="3" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="B22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1101,90 +1129,90 @@
       <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="B23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="1"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="B24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="1"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="1"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" s="4" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" s="3" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="B28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="7" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1192,84 +1220,89 @@
       <c r="A29" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="B29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="1"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="B30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="1"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="B31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="1"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="7"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="B32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="1"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="7"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="B33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="1"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="F15:F17"/>
     <mergeCell ref="E28:E33"/>
     <mergeCell ref="F28:F33"/>
@@ -1277,15 +1310,13 @@
     <mergeCell ref="E12:E17"/>
     <mergeCell ref="E22:E26"/>
     <mergeCell ref="F22:F26"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
     <mergeCell ref="F6:F8"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C10" r:id="rId1" xr:uid="{4A58428B-2E9C-4561-A0A9-8E742BC17592}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="landscape" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>